<commit_message>
same version. office machine
</commit_message>
<xml_diff>
--- a/Data/SPMECalibration.xlsx
+++ b/Data/SPMECalibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/martie_uiowa_edu/Documents/Work/ISRP/Project5/David/PCB-Aerobic-Bioaugmentation-Study2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{4EE1E9E6-BFE4-814F-8974-9B033E39AFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{962332E3-6148-4D96-AF4D-F65F7DEB71FC}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{4EE1E9E6-BFE4-814F-8974-9B033E39AFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3D54695-B322-4CC5-8917-71448FF77354}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{828D58CB-7CD6-D040-BD0A-8E8F0158FC2C}"/>
+    <workbookView xWindow="8710" yWindow="1870" windowWidth="28800" windowHeight="15370" activeTab="5" xr2:uid="{828D58CB-7CD6-D040-BD0A-8E8F0158FC2C}"/>
   </bookViews>
   <sheets>
     <sheet name="day5_14" sheetId="1" r:id="rId1"/>
@@ -24479,14 +24479,10 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -24524,7 +24520,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -24630,7 +24626,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -24772,7 +24768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -24784,9 +24780,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>[1]DataR!A1</f>
         <v>sample</v>
@@ -25368,7 +25364,7 @@
         <v>PCB181</v>
       </c>
     </row>
-    <row r="2" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>[1]DataR!A2</f>
         <v>S01</v>
@@ -25950,7 +25946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>[1]DataR!A3</f>
         <v>S02</v>
@@ -26532,7 +26528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>[1]DataR!A4</f>
         <v>S03</v>
@@ -27114,7 +27110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>[1]DataR!A5</f>
         <v>S04</v>
@@ -27696,7 +27692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>[1]DataR!A6</f>
         <v>S05</v>
@@ -28278,7 +28274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>[1]DataR!A7</f>
         <v>S06</v>
@@ -28860,7 +28856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>[1]DataR!A8</f>
         <v>S07</v>
@@ -29442,7 +29438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>[1]DataR!A9</f>
         <v>S08</v>
@@ -30024,7 +30020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>[1]DataR!A10</f>
         <v>S09</v>
@@ -30606,7 +30602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>[1]DataR!A11</f>
         <v>S10</v>
@@ -31188,7 +31184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>+[2]DataR!A2</f>
         <v>S01</v>
@@ -31770,7 +31766,7 @@
         <v>0.14797752920212087</v>
       </c>
     </row>
-    <row r="13" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>+[2]DataR!A3</f>
         <v>S02</v>
@@ -32365,9 +32361,9 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>[3]DataR!A1</f>
         <v>sample</v>
@@ -32949,7 +32945,7 @@
         <v>PCB181</v>
       </c>
     </row>
-    <row r="2" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>[3]DataR!A2</f>
         <v>S01</v>
@@ -33531,7 +33527,7 @@
         <v>0.10694883324771126</v>
       </c>
     </row>
-    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>[3]DataR!A3</f>
         <v>S02</v>
@@ -34113,7 +34109,7 @@
         <v>0.13789242416621908</v>
       </c>
     </row>
-    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>[3]DataR!A4</f>
         <v>S03</v>
@@ -34695,7 +34691,7 @@
         <v>8.7042045655471315E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>[3]DataR!A5</f>
         <v>S04</v>
@@ -35277,7 +35273,7 @@
         <v>0.13179355002577214</v>
       </c>
     </row>
-    <row r="6" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>[3]DataR!A6</f>
         <v>S05</v>
@@ -35859,7 +35855,7 @@
         <v>0.12626877120343458</v>
       </c>
     </row>
-    <row r="7" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>+[4]DataR!A2</f>
         <v>S01</v>
@@ -36454,9 +36450,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>[5]DataR!A1</f>
         <v>sample</v>
@@ -37038,7 +37034,7 @@
         <v>PCB181</v>
       </c>
     </row>
-    <row r="2" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>[5]DataR!A2</f>
         <v>S01</v>
@@ -37620,7 +37616,7 @@
         <v>5.6730592296581291E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>[5]DataR!A3</f>
         <v>S02</v>
@@ -38202,7 +38198,7 @@
         <v>0.10046671962643959</v>
       </c>
     </row>
-    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>[5]DataR!A4</f>
         <v>S03</v>
@@ -38784,7 +38780,7 @@
         <v>6.4562055385715064E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>[5]DataR!A5</f>
         <v>S04</v>
@@ -39366,7 +39362,7 @@
         <v>4.4583531765985999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>[5]DataR!A6</f>
         <v>S05</v>
@@ -39948,7 +39944,7 @@
         <v>8.1692052907077067E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>+[4]DataR!A3</f>
         <v>S02</v>
@@ -40543,9 +40539,9 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>[6]DataR!A1</f>
         <v>sample</v>
@@ -41259,7 +41255,7 @@
         <v>PCB209</v>
       </c>
     </row>
-    <row r="2" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>[6]DataR!A2</f>
         <v>16_1</v>
@@ -41973,7 +41969,7 @@
         <v>0.2068188294659267</v>
       </c>
     </row>
-    <row r="3" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>[6]DataR!A3</f>
         <v>16_2</v>
@@ -42687,7 +42683,7 @@
         <v>0.20215235424493547</v>
       </c>
     </row>
-    <row r="4" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>[6]DataR!A4</f>
         <v>16_3</v>
@@ -43401,7 +43397,7 @@
         <v>0.19792519433113151</v>
       </c>
     </row>
-    <row r="5" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>[6]DataR!A5</f>
         <v>35_1</v>
@@ -44115,7 +44111,7 @@
         <v>0.18917018402776387</v>
       </c>
     </row>
-    <row r="6" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>[6]DataR!A6</f>
         <v>35_2</v>
@@ -44829,7 +44825,7 @@
         <v>0.19137985329856266</v>
       </c>
     </row>
-    <row r="7" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>[6]DataR!A7</f>
         <v>35_3</v>
@@ -45543,7 +45539,7 @@
         <v>0.17253284514187192</v>
       </c>
     </row>
-    <row r="8" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>[6]DataR!A8</f>
         <v>75_1</v>
@@ -46257,7 +46253,7 @@
         <v>0.17839219590335398</v>
       </c>
     </row>
-    <row r="9" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>[6]DataR!A9</f>
         <v>75_2</v>
@@ -46971,7 +46967,7 @@
         <v>0.20164151963791707</v>
       </c>
     </row>
-    <row r="10" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>[6]DataR!A10</f>
         <v>75_3</v>
@@ -47694,13 +47690,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD116596-1288-9A47-8082-CC3E7249B49B}">
   <dimension ref="A1:FV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>[7]DataR!A1</f>
         <v>sample</v>
@@ -48414,7 +48410,7 @@
         <v>PCB209</v>
       </c>
     </row>
-    <row r="2" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>[7]DataR!A2</f>
         <v>3_1</v>
@@ -49128,7 +49124,7 @@
         <v>3.1964925319526091E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>[7]DataR!A3</f>
         <v>3_2</v>
@@ -49842,7 +49838,7 @@
         <v>3.9025975612221125E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>[7]DataR!A4</f>
         <v>3_3</v>
@@ -50556,7 +50552,7 @@
         <v>3.457920174083897E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>[7]DataR!A5</f>
         <v>11_1</v>
@@ -51270,7 +51266,7 @@
         <v>5.1501772629506545E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>[7]DataR!A6</f>
         <v>11_2</v>
@@ -51984,7 +51980,7 @@
         <v>4.3149368602181402E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>[7]DataR!A7</f>
         <v>11_3</v>
@@ -52698,7 +52694,7 @@
         <v>4.0917684057008623E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>[7]DataR!A8</f>
         <v>16_1</v>
@@ -53412,7 +53408,7 @@
         <v>5.1696540921685678E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>[7]DataR!A9</f>
         <v>16_2</v>
@@ -54126,7 +54122,7 @@
         <v>4.1356011652889872E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>[7]DataR!A10</f>
         <v>16_3</v>
@@ -54840,7 +54836,7 @@
         <v>5.7714737799829142E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>[7]DataR!A11</f>
         <v>35_1</v>
@@ -55554,7 +55550,7 @@
         <v>2.4065792236417503E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>[7]DataR!A12</f>
         <v>35_2</v>
@@ -56268,7 +56264,7 @@
         <v>4.2075159524579783E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:178" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>[7]DataR!A13</f>
         <v>35_3</v>
@@ -56991,13 +56987,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBBB7F-67FF-4F4E-9E8E-FC97F3A8AFF6}">
   <dimension ref="A1:EO25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>+day5_14!A1</f>
         <v>sample</v>
@@ -57579,7 +57575,7 @@
         <v>PCB181</v>
       </c>
     </row>
-    <row r="2" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>+day5_14!A2</f>
         <v>S01</v>
@@ -58161,7 +58157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>+day5_14!A3</f>
         <v>S02</v>
@@ -58743,7 +58739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>+day5_14!A4</f>
         <v>S03</v>
@@ -59325,7 +59321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>+day5_14!A5</f>
         <v>S04</v>
@@ -59907,7 +59903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>+day5_14!A6</f>
         <v>S05</v>
@@ -60489,7 +60485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>+day5_14!A7</f>
         <v>S06</v>
@@ -61071,7 +61067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>+day5_14!A8</f>
         <v>S07</v>
@@ -61653,7 +61649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>+day5_14!A9</f>
         <v>S08</v>
@@ -62235,7 +62231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>+day5_14!A10</f>
         <v>S09</v>
@@ -62817,7 +62813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>+day5_14!A11</f>
         <v>S10</v>
@@ -63399,7 +63395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>+day5_14!A12</f>
         <v>S01</v>
@@ -63981,7 +63977,7 @@
         <v>0.14797752920212087</v>
       </c>
     </row>
-    <row r="13" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>+day5_14!A13</f>
         <v>S02</v>
@@ -64563,7 +64559,7 @@
         <v>0.13626958567902198</v>
       </c>
     </row>
-    <row r="14" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f>+'day42'!A2</f>
         <v>S01</v>
@@ -65145,7 +65141,7 @@
         <v>0.10694883324771126</v>
       </c>
     </row>
-    <row r="15" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>+'day42'!A3</f>
         <v>S02</v>
@@ -65727,7 +65723,7 @@
         <v>0.13789242416621908</v>
       </c>
     </row>
-    <row r="16" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>+'day42'!A4</f>
         <v>S03</v>
@@ -66309,7 +66305,7 @@
         <v>8.7042045655471315E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>+'day42'!A5</f>
         <v>S04</v>
@@ -66891,7 +66887,7 @@
         <v>0.13179355002577214</v>
       </c>
     </row>
-    <row r="18" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>+'day42'!A6</f>
         <v>S05</v>
@@ -67473,7 +67469,7 @@
         <v>0.12626877120343458</v>
       </c>
     </row>
-    <row r="19" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>+'day42'!A7</f>
         <v>S01</v>
@@ -68055,7 +68051,7 @@
         <v>5.6899108049286287E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>+'day85'!A2</f>
         <v>S01</v>
@@ -68637,7 +68633,7 @@
         <v>5.6730592296581291E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>+'day85'!A3</f>
         <v>S02</v>
@@ -69219,7 +69215,7 @@
         <v>0.10046671962643959</v>
       </c>
     </row>
-    <row r="22" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>+'day85'!A4</f>
         <v>S03</v>
@@ -69801,7 +69797,7 @@
         <v>6.4562055385715064E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>+'day85'!A5</f>
         <v>S04</v>
@@ -70383,7 +70379,7 @@
         <v>4.4583531765985999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>+'day85'!A6</f>
         <v>S05</v>
@@ -70965,7 +70961,7 @@
         <v>8.1692052907077067E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>+'day85'!A7</f>
         <v>S02</v>

</xml_diff>

<commit_message>
same version, mac  machine
</commit_message>
<xml_diff>
--- a/Data/SPMECalibration.xlsx
+++ b/Data/SPMECalibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/martie_uiowa_edu/Documents/Work/ISRP/Project5/David/PCB-Aerobic-Bioaugmentation-Study2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{4EE1E9E6-BFE4-814F-8974-9B033E39AFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3D54695-B322-4CC5-8917-71448FF77354}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{4EE1E9E6-BFE4-814F-8974-9B033E39AFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09FED7C3-3FAE-4809-BA56-97D20B01924D}"/>
   <bookViews>
-    <workbookView xWindow="8710" yWindow="1870" windowWidth="28800" windowHeight="15370" activeTab="5" xr2:uid="{828D58CB-7CD6-D040-BD0A-8E8F0158FC2C}"/>
+    <workbookView xWindow="5830" yWindow="1200" windowWidth="28800" windowHeight="18780" activeTab="5" xr2:uid="{828D58CB-7CD6-D040-BD0A-8E8F0158FC2C}"/>
   </bookViews>
   <sheets>
     <sheet name="day5_14" sheetId="1" r:id="rId1"/>
@@ -99,6 +99,1073 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$K$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$D$2:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$T$2:$T$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>5.7518930010701137</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7857043715981042</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0918489802748148</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9080414456746162</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.659089671830523</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8977210175910812</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8031798196493645</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5317869015506327</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9328809123040624</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.8007067230881511</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.41346245009109767</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.27535977225139757</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0591370232304111</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.3261796870646547</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8578922712067332</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.2025422878567191</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.751022487691472</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26811610003059727</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.0305490356671516</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.600664180598825</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.2224558195497917</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5299307031057197</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.58862880155176</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.55781011899947486</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C8A-43B5-A5EA-923550F93035}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="249952351"/>
+        <c:axId val="249954751"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="249952351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="249954751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="249954751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="249952351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>143566</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>33682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>77305</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>192708</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90CDE02A-F0DA-3676-C578-A4A61A24511D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -24477,6 +25544,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56987,8 +58058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DBBB7F-67FF-4F4E-9E8E-FC97F3A8AFF6}">
   <dimension ref="A1:EO25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -71545,5 +72616,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>